<commit_message>
Escritura en Excel original e Integración con la UI (parcial)
Falta control de excepciones
</commit_message>
<xml_diff>
--- a/precios_finales.xlsx
+++ b/precios_finales.xlsx
@@ -525,17 +525,17 @@
         <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>388.4297521</v>
+        <v>0</v>
       </c>
       <c r="J2" t="n">
         <v>471.7719518</v>
       </c>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="n">
-        <v>470</v>
+        <v>0</v>
       </c>
       <c r="M2" t="n">
-        <v>470</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -568,17 +568,17 @@
         <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>132.231405</v>
+        <v>0</v>
       </c>
       <c r="J3" t="n">
         <v>159.4345005</v>
       </c>
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="n">
-        <v>160</v>
+        <v>0</v>
       </c>
       <c r="M3" t="n">
-        <v>160</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -611,17 +611,17 @@
         <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>148.7603306</v>
+        <v>0</v>
       </c>
       <c r="J4" t="n">
         <v>177.492843</v>
       </c>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="n">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="M4" t="n">
-        <v>180</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -654,17 +654,17 @@
         <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>181.8181818</v>
+        <v>0</v>
       </c>
       <c r="J5" t="n">
         <v>218.5957868</v>
       </c>
       <c r="K5" t="inlineStr"/>
       <c r="L5" t="n">
-        <v>220</v>
+        <v>0</v>
       </c>
       <c r="M5" t="n">
-        <v>220</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -697,17 +697,17 @@
         <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>181.8181818</v>
+        <v>8.264462809999999</v>
       </c>
       <c r="J6" t="n">
         <v>223.9773525</v>
       </c>
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="n">
-        <v>220</v>
+        <v>10</v>
       </c>
       <c r="M6" t="n">
-        <v>220</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7">
@@ -740,17 +740,17 @@
         <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>190.0826446</v>
+        <v>8.264462809999999</v>
       </c>
       <c r="J7" t="n">
         <v>229.745241</v>
       </c>
       <c r="K7" t="inlineStr"/>
       <c r="L7" t="n">
-        <v>230</v>
+        <v>10</v>
       </c>
       <c r="M7" t="n">
-        <v>230</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8">
@@ -783,17 +783,17 @@
         <v>0</v>
       </c>
       <c r="I8" t="n">
-        <v>206.6115702</v>
+        <v>8.264462809999999</v>
       </c>
       <c r="J8" t="n">
         <v>247.4172608</v>
       </c>
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="n">
-        <v>250</v>
+        <v>10</v>
       </c>
       <c r="M8" t="n">
-        <v>250</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9">
@@ -826,17 +826,17 @@
         <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>206.6115702</v>
+        <v>8.264462809999999</v>
       </c>
       <c r="J9" t="n">
         <v>248.9535675</v>
       </c>
       <c r="K9" t="inlineStr"/>
       <c r="L9" t="n">
-        <v>250</v>
+        <v>10</v>
       </c>
       <c r="M9" t="n">
-        <v>250</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10">
@@ -869,17 +869,17 @@
         <v>0</v>
       </c>
       <c r="I10" t="n">
-        <v>214.8760331</v>
+        <v>8.264462809999999</v>
       </c>
       <c r="J10" t="n">
         <v>256.6351013</v>
       </c>
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="n">
-        <v>260</v>
+        <v>10</v>
       </c>
       <c r="M10" t="n">
-        <v>260</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11">
@@ -912,17 +912,17 @@
         <v>0</v>
       </c>
       <c r="I11" t="n">
-        <v>214.8760331</v>
+        <v>8.264462809999999</v>
       </c>
       <c r="J11" t="n">
         <v>263.166651</v>
       </c>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="n">
-        <v>260</v>
+        <v>10</v>
       </c>
       <c r="M11" t="n">
-        <v>260</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12">
@@ -955,17 +955,17 @@
         <v>0</v>
       </c>
       <c r="I12" t="n">
-        <v>223.1404959</v>
+        <v>0</v>
       </c>
       <c r="J12" t="n">
         <v>270.0845235</v>
       </c>
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="n">
-        <v>270</v>
+        <v>0</v>
       </c>
       <c r="M12" t="n">
-        <v>270</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -998,17 +998,17 @@
         <v>0</v>
       </c>
       <c r="I13" t="n">
-        <v>231.4049587</v>
+        <v>8.264462809999999</v>
       </c>
       <c r="J13" t="n">
         <v>276.2297505</v>
       </c>
       <c r="K13" t="inlineStr"/>
       <c r="L13" t="n">
-        <v>280</v>
+        <v>10</v>
       </c>
       <c r="M13" t="n">
-        <v>280</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14">
@@ -1041,17 +1041,17 @@
         <v>0</v>
       </c>
       <c r="I14" t="n">
-        <v>231.4049587</v>
+        <v>8.264462809999999</v>
       </c>
       <c r="J14" t="n">
         <v>281.9886548</v>
       </c>
       <c r="K14" t="inlineStr"/>
       <c r="L14" t="n">
-        <v>280</v>
+        <v>10</v>
       </c>
       <c r="M14" t="n">
-        <v>280</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15">
@@ -1084,17 +1084,17 @@
         <v>0</v>
       </c>
       <c r="I15" t="n">
-        <v>231.4049587</v>
+        <v>8.264462809999999</v>
       </c>
       <c r="J15" t="n">
         <v>281.9886548</v>
       </c>
       <c r="K15" t="inlineStr"/>
       <c r="L15" t="n">
-        <v>280</v>
+        <v>10</v>
       </c>
       <c r="M15" t="n">
-        <v>280</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16">
@@ -1127,15 +1127,15 @@
         <v>0</v>
       </c>
       <c r="I16" t="n">
-        <v>190.0826446</v>
+        <v>8.264462809999999</v>
       </c>
       <c r="J16" t="inlineStr"/>
       <c r="K16" t="inlineStr"/>
       <c r="L16" t="n">
-        <v>230</v>
+        <v>10</v>
       </c>
       <c r="M16" t="n">
-        <v>230</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17">
@@ -1168,15 +1168,15 @@
         <v>0</v>
       </c>
       <c r="I17" t="n">
-        <v>66.11570248</v>
+        <v>8.264462809999999</v>
       </c>
       <c r="J17" t="inlineStr"/>
       <c r="K17" t="inlineStr"/>
       <c r="L17" t="n">
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="M17" t="n">
-        <v>80</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18">
@@ -1209,15 +1209,15 @@
         <v>0</v>
       </c>
       <c r="I18" t="n">
-        <v>140.4958678</v>
+        <v>8.264462809999999</v>
       </c>
       <c r="J18" t="inlineStr"/>
       <c r="K18" t="inlineStr"/>
       <c r="L18" t="n">
-        <v>170</v>
+        <v>10</v>
       </c>
       <c r="M18" t="n">
-        <v>170</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19">
@@ -1250,15 +1250,15 @@
         <v>0</v>
       </c>
       <c r="I19" t="n">
-        <v>256.1983471</v>
+        <v>8.264462809999999</v>
       </c>
       <c r="J19" t="inlineStr"/>
       <c r="K19" t="inlineStr"/>
       <c r="L19" t="n">
-        <v>310</v>
+        <v>10</v>
       </c>
       <c r="M19" t="n">
-        <v>310</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20">
@@ -1291,15 +1291,15 @@
         <v>0</v>
       </c>
       <c r="I20" t="n">
-        <v>90.90909091</v>
+        <v>8.264462809999999</v>
       </c>
       <c r="J20" t="inlineStr"/>
       <c r="K20" t="inlineStr"/>
       <c r="L20" t="n">
-        <v>110</v>
+        <v>10</v>
       </c>
       <c r="M20" t="n">
-        <v>110</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21">
@@ -1332,15 +1332,15 @@
         <v>0</v>
       </c>
       <c r="I21" t="n">
-        <v>157.0247934</v>
+        <v>8.264462809999999</v>
       </c>
       <c r="J21" t="inlineStr"/>
       <c r="K21" t="inlineStr"/>
       <c r="L21" t="n">
-        <v>190</v>
+        <v>10</v>
       </c>
       <c r="M21" t="n">
-        <v>190</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22">
@@ -1373,15 +1373,15 @@
         <v>0</v>
       </c>
       <c r="I22" t="n">
-        <v>82.64462810000001</v>
+        <v>8.264462809999999</v>
       </c>
       <c r="J22" t="inlineStr"/>
       <c r="K22" t="inlineStr"/>
       <c r="L22" t="n">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="M22" t="n">
-        <v>100</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23">
@@ -1414,15 +1414,15 @@
         <v>0</v>
       </c>
       <c r="I23" t="n">
-        <v>132.231405</v>
+        <v>8.264462809999999</v>
       </c>
       <c r="J23" t="inlineStr"/>
       <c r="K23" t="inlineStr"/>
       <c r="L23" t="n">
-        <v>160</v>
+        <v>10</v>
       </c>
       <c r="M23" t="n">
-        <v>160</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24">
@@ -1455,15 +1455,15 @@
         <v>0</v>
       </c>
       <c r="I24" t="n">
-        <v>132.231405</v>
+        <v>0</v>
       </c>
       <c r="J24" t="inlineStr"/>
       <c r="K24" t="inlineStr"/>
       <c r="L24" t="n">
-        <v>160</v>
+        <v>0</v>
       </c>
       <c r="M24" t="n">
-        <v>160</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -1496,15 +1496,15 @@
         <v>0</v>
       </c>
       <c r="I25" t="n">
-        <v>74.38016528999999</v>
+        <v>8.264462809999999</v>
       </c>
       <c r="J25" t="inlineStr"/>
       <c r="K25" t="inlineStr"/>
       <c r="L25" t="n">
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="M25" t="n">
-        <v>90</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26">
@@ -1537,15 +1537,15 @@
         <v>0</v>
       </c>
       <c r="I26" t="n">
-        <v>41.32231405</v>
+        <v>8.264462809999999</v>
       </c>
       <c r="J26" t="inlineStr"/>
       <c r="K26" t="inlineStr"/>
       <c r="L26" t="n">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="M26" t="n">
-        <v>50</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27">
@@ -1578,15 +1578,15 @@
         <v>0</v>
       </c>
       <c r="I27" t="n">
-        <v>49.58677686</v>
+        <v>8.264462809999999</v>
       </c>
       <c r="J27" t="inlineStr"/>
       <c r="K27" t="inlineStr"/>
       <c r="L27" t="n">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="M27" t="n">
-        <v>60</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28">
@@ -1619,15 +1619,15 @@
         <v>0</v>
       </c>
       <c r="I28" t="n">
-        <v>181.8181818</v>
+        <v>0</v>
       </c>
       <c r="J28" t="inlineStr"/>
       <c r="K28" t="inlineStr"/>
       <c r="L28" t="n">
-        <v>220</v>
+        <v>0</v>
       </c>
       <c r="M28" t="n">
-        <v>220</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29">
@@ -1660,15 +1660,15 @@
         <v>0</v>
       </c>
       <c r="I29" t="n">
-        <v>181.8181818</v>
+        <v>8.264462809999999</v>
       </c>
       <c r="J29" t="inlineStr"/>
       <c r="K29" t="inlineStr"/>
       <c r="L29" t="n">
-        <v>220</v>
+        <v>10</v>
       </c>
       <c r="M29" t="n">
-        <v>220</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30">
@@ -1701,15 +1701,15 @@
         <v>0</v>
       </c>
       <c r="I30" t="n">
-        <v>165.2892562</v>
+        <v>8.264462809999999</v>
       </c>
       <c r="J30" t="inlineStr"/>
       <c r="K30" t="inlineStr"/>
       <c r="L30" t="n">
-        <v>200</v>
+        <v>10</v>
       </c>
       <c r="M30" t="n">
-        <v>200</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31">
@@ -1742,15 +1742,15 @@
         <v>0</v>
       </c>
       <c r="I31" t="n">
-        <v>181.8181818</v>
+        <v>8.264462809999999</v>
       </c>
       <c r="J31" t="inlineStr"/>
       <c r="K31" t="inlineStr"/>
       <c r="L31" t="n">
-        <v>220</v>
+        <v>10</v>
       </c>
       <c r="M31" t="n">
-        <v>220</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32">
@@ -1783,15 +1783,15 @@
         <v>0</v>
       </c>
       <c r="I32" t="n">
-        <v>157.0247934</v>
+        <v>8.264462809999999</v>
       </c>
       <c r="J32" t="inlineStr"/>
       <c r="K32" t="inlineStr"/>
       <c r="L32" t="n">
-        <v>190</v>
+        <v>10</v>
       </c>
       <c r="M32" t="n">
-        <v>190</v>
+        <v>10</v>
       </c>
     </row>
     <row r="33">
@@ -1824,15 +1824,15 @@
         <v>0</v>
       </c>
       <c r="I33" t="n">
-        <v>115.7024793</v>
+        <v>8.264462809999999</v>
       </c>
       <c r="J33" t="inlineStr"/>
       <c r="K33" t="inlineStr"/>
       <c r="L33" t="n">
-        <v>140</v>
+        <v>10</v>
       </c>
       <c r="M33" t="n">
-        <v>140</v>
+        <v>10</v>
       </c>
     </row>
     <row r="34">
@@ -1865,15 +1865,15 @@
         <v>0</v>
       </c>
       <c r="I34" t="n">
-        <v>115.7024793</v>
+        <v>8.264462809999999</v>
       </c>
       <c r="J34" t="inlineStr"/>
       <c r="K34" t="inlineStr"/>
       <c r="L34" t="n">
-        <v>140</v>
+        <v>10</v>
       </c>
       <c r="M34" t="n">
-        <v>140</v>
+        <v>10</v>
       </c>
     </row>
     <row r="35">
@@ -1906,15 +1906,15 @@
         <v>0</v>
       </c>
       <c r="I35" t="n">
-        <v>90.90909091</v>
+        <v>8.264462809999999</v>
       </c>
       <c r="J35" t="inlineStr"/>
       <c r="K35" t="inlineStr"/>
       <c r="L35" t="n">
-        <v>110</v>
+        <v>10</v>
       </c>
       <c r="M35" t="n">
-        <v>110</v>
+        <v>10</v>
       </c>
     </row>
     <row r="36">
@@ -1947,15 +1947,15 @@
         <v>0</v>
       </c>
       <c r="I36" t="n">
-        <v>115.7024793</v>
+        <v>0</v>
       </c>
       <c r="J36" t="inlineStr"/>
       <c r="K36" t="inlineStr"/>
       <c r="L36" t="n">
-        <v>140</v>
+        <v>0</v>
       </c>
       <c r="M36" t="n">
-        <v>140</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37">
@@ -1988,15 +1988,15 @@
         <v>0</v>
       </c>
       <c r="I37" t="n">
-        <v>90.90909091</v>
+        <v>8.264462809999999</v>
       </c>
       <c r="J37" t="inlineStr"/>
       <c r="K37" t="inlineStr"/>
       <c r="L37" t="n">
-        <v>110</v>
+        <v>10</v>
       </c>
       <c r="M37" t="n">
-        <v>110</v>
+        <v>10</v>
       </c>
     </row>
     <row r="38">
@@ -2029,15 +2029,15 @@
         <v>0</v>
       </c>
       <c r="I38" t="n">
-        <v>173.553719</v>
+        <v>0</v>
       </c>
       <c r="J38" t="inlineStr"/>
       <c r="K38" t="inlineStr"/>
       <c r="L38" t="n">
-        <v>210</v>
+        <v>0</v>
       </c>
       <c r="M38" t="n">
-        <v>210</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39">
@@ -2070,15 +2070,15 @@
         <v>0</v>
       </c>
       <c r="I39" t="n">
-        <v>107.4380165</v>
+        <v>8.264462809999999</v>
       </c>
       <c r="J39" t="inlineStr"/>
       <c r="K39" t="inlineStr"/>
       <c r="L39" t="n">
-        <v>130</v>
+        <v>10</v>
       </c>
       <c r="M39" t="n">
-        <v>130</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40">
@@ -2111,15 +2111,15 @@
         <v>0</v>
       </c>
       <c r="I40" t="n">
-        <v>132.231405</v>
+        <v>0</v>
       </c>
       <c r="J40" t="inlineStr"/>
       <c r="K40" t="inlineStr"/>
       <c r="L40" t="n">
-        <v>160</v>
+        <v>0</v>
       </c>
       <c r="M40" t="n">
-        <v>160</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41">
@@ -2152,15 +2152,15 @@
         <v>0</v>
       </c>
       <c r="I41" t="n">
-        <v>41.32231405</v>
+        <v>8.264462809999999</v>
       </c>
       <c r="J41" t="inlineStr"/>
       <c r="K41" t="inlineStr"/>
       <c r="L41" t="n">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="M41" t="n">
-        <v>50</v>
+        <v>10</v>
       </c>
     </row>
     <row r="42">
@@ -2193,15 +2193,15 @@
         <v>0</v>
       </c>
       <c r="I42" t="n">
-        <v>49.58677686</v>
+        <v>8.264462809999999</v>
       </c>
       <c r="J42" t="inlineStr"/>
       <c r="K42" t="inlineStr"/>
       <c r="L42" t="n">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="M42" t="n">
-        <v>60</v>
+        <v>10</v>
       </c>
     </row>
     <row r="43">
@@ -2234,15 +2234,15 @@
         <v>0</v>
       </c>
       <c r="I43" t="n">
-        <v>107.4380165</v>
+        <v>8.264462809999999</v>
       </c>
       <c r="J43" t="inlineStr"/>
       <c r="K43" t="inlineStr"/>
       <c r="L43" t="n">
-        <v>130</v>
+        <v>10</v>
       </c>
       <c r="M43" t="n">
-        <v>130</v>
+        <v>10</v>
       </c>
     </row>
     <row r="44">
@@ -2275,15 +2275,15 @@
         <v>0</v>
       </c>
       <c r="I44" t="n">
-        <v>289.2561983</v>
+        <v>8.264462809999999</v>
       </c>
       <c r="J44" t="inlineStr"/>
       <c r="K44" t="inlineStr"/>
       <c r="L44" t="n">
-        <v>350</v>
+        <v>10</v>
       </c>
       <c r="M44" t="n">
-        <v>350</v>
+        <v>10</v>
       </c>
     </row>
     <row r="45">
@@ -2316,15 +2316,15 @@
         <v>0</v>
       </c>
       <c r="I45" t="n">
-        <v>190.0826446</v>
+        <v>8.264462809999999</v>
       </c>
       <c r="J45" t="inlineStr"/>
       <c r="K45" t="inlineStr"/>
       <c r="L45" t="n">
-        <v>230</v>
+        <v>10</v>
       </c>
       <c r="M45" t="n">
-        <v>230</v>
+        <v>10</v>
       </c>
     </row>
     <row r="46">
@@ -2357,15 +2357,15 @@
         <v>0</v>
       </c>
       <c r="I46" t="n">
-        <v>206.6115702</v>
+        <v>8.264462809999999</v>
       </c>
       <c r="J46" t="inlineStr"/>
       <c r="K46" t="inlineStr"/>
       <c r="L46" t="n">
-        <v>250</v>
+        <v>10</v>
       </c>
       <c r="M46" t="n">
-        <v>250</v>
+        <v>10</v>
       </c>
     </row>
     <row r="47">
@@ -2398,15 +2398,15 @@
         <v>0</v>
       </c>
       <c r="I47" t="n">
-        <v>487.6033058</v>
+        <v>8.264462809999999</v>
       </c>
       <c r="J47" t="inlineStr"/>
       <c r="K47" t="inlineStr"/>
       <c r="L47" t="n">
-        <v>590</v>
+        <v>10</v>
       </c>
       <c r="M47" t="n">
-        <v>590</v>
+        <v>10</v>
       </c>
     </row>
     <row r="48">
@@ -2439,15 +2439,15 @@
         <v>0</v>
       </c>
       <c r="I48" t="n">
-        <v>305.785124</v>
+        <v>0</v>
       </c>
       <c r="J48" t="inlineStr"/>
       <c r="K48" t="inlineStr"/>
       <c r="L48" t="n">
-        <v>370</v>
+        <v>0</v>
       </c>
       <c r="M48" t="n">
-        <v>370</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49">
@@ -2480,15 +2480,15 @@
         <v>0</v>
       </c>
       <c r="I49" t="n">
-        <v>404.9586777</v>
+        <v>0</v>
       </c>
       <c r="J49" t="inlineStr"/>
       <c r="K49" t="inlineStr"/>
       <c r="L49" t="n">
-        <v>490</v>
+        <v>0</v>
       </c>
       <c r="M49" t="n">
-        <v>490</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50">
@@ -2521,15 +2521,15 @@
         <v>0</v>
       </c>
       <c r="I50" t="n">
-        <v>90.90909091</v>
+        <v>8.264462809999999</v>
       </c>
       <c r="J50" t="inlineStr"/>
       <c r="K50" t="inlineStr"/>
       <c r="L50" t="n">
-        <v>110</v>
+        <v>10</v>
       </c>
       <c r="M50" t="n">
-        <v>110</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>